<commit_message>
all files are added and finalized
</commit_message>
<xml_diff>
--- a/data/MT_test_submission_with_predcitions.xlsx
+++ b/data/MT_test_submission_with_predcitions.xlsx
@@ -397,7 +397,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1010.any(3)</t>
+          <t>1010.any()</t>
         </is>
       </c>
     </row>
@@ -417,7 +417,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>q11.any(5)</t>
+          <t>.any(5)</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1.any(&lt;DGT0&gt;)</t>
+          <t>1.any()</t>
         </is>
       </c>
     </row>
@@ -795,7 +795,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>qr7.any(1)&amp;qr7.any(1)</t>
+          <t>q30.any(1)&amp;q30.any(4)</t>
         </is>
       </c>
     </row>
@@ -835,7 +835,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2302b.notany(7)</t>
+          <t>q2302b.any(7)</t>
         </is>
       </c>
     </row>
@@ -895,7 +895,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1.any(2)</t>
+          <t>q43.any(2)</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1251.notanswered(1)</t>
+          <t>1251.answered(1)</t>
         </is>
       </c>
     </row>
@@ -990,11 +990,7 @@
           <t>END Younger than 18 years</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>8014&lt;18</t>
-        </is>
-      </c>
+      <c r="D32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1013,7 +1009,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>–.any(51021)</t>
+          <t>–.answered()</t>
         </is>
       </c>
     </row>
@@ -1033,7 +1029,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>s2.notany(5,6,7)</t>
+          <t>s2.notany(5,6)</t>
         </is>
       </c>
     </row>
@@ -1073,7 +1069,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>question12.any(1,2)</t>
+          <t>.any(1,2)</t>
         </is>
       </c>
     </row>
@@ -1093,7 +1089,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>21993.any(&lt;DGT0&gt;,&lt;DGT1&gt;)</t>
+          <t>21993.any(,)</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1107,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1700.answered()</t>
+          <t>.answered(1)</t>
         </is>
       </c>
     </row>
@@ -1131,7 +1127,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -1171,7 +1167,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>q32600.any(&lt;DGT0&gt;)</t>
+          <t>q32600.any()</t>
         </is>
       </c>
     </row>
@@ -1209,11 +1205,7 @@
           <t>[PN: ONLY ASK IF GREATER THAN 0 IN Q16. OTHERWISE, SKIP TO Q18]</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>q17 q18.any(0)</t>
-        </is>
-      </c>
+      <c r="D43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1311,7 +1303,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -1349,7 +1341,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1015.any(&lt;DGT0&gt;)</t>
+          <t>1015.any()</t>
         </is>
       </c>
     </row>
@@ -1369,7 +1361,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>42061.any(1,4230)</t>
+          <t>42061.any(1)</t>
         </is>
       </c>
     </row>
@@ -1409,7 +1401,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>q15a.between(1:4)</t>
+          <t>qd.between(1:4)</t>
         </is>
       </c>
     </row>
@@ -1429,7 +1421,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>q12.any(2)</t>
+          <t>qa1.any(2)</t>
         </is>
       </c>
     </row>
@@ -1469,7 +1461,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>&lt;QID3&gt;.any(&lt;DGT0&gt;)or q99010.</t>
+          <t>q1002.any()</t>
         </is>
       </c>
     </row>
@@ -1529,7 +1521,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>q0020b.any(&lt;DGT0&gt;)</t>
+          <t>q0020b.any()</t>
         </is>
       </c>
     </row>
@@ -1609,7 +1601,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>.any(&lt;DGT0&gt;)</t>
+          <t>.any()</t>
         </is>
       </c>
     </row>
@@ -1649,7 +1641,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>qc1.any(1,2)</t>
+          <t>qa1.any(1,2,3)</t>
         </is>
       </c>
     </row>
@@ -1729,7 +1721,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>q12.any(2)</t>
+          <t>qa1.any(2)</t>
         </is>
       </c>
     </row>
@@ -1827,7 +1819,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>1100003.any(&lt;DGT0&gt;)</t>
+          <t>1100003.any()</t>
         </is>
       </c>
     </row>
@@ -1847,7 +1839,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>qa.any(1)&amp;qh1.between.between(6</t>
+          <t>qa.any(1)&amp;qa.any(6)</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1939,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>s5.any(2,35)</t>
+          <t>s5 &lt;2 or s5 &gt;35</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2019,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2302b.notany(3)</t>
+          <t>q2202.any(3)</t>
         </is>
       </c>
     </row>
@@ -2227,7 +2219,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>q51.any(1)&amp;.between.any(&lt;DGT1&gt;)</t>
+          <t>q46.any(1)q49</t>
         </is>
       </c>
     </row>
@@ -2247,7 +2239,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>&lt;DGT2&gt;.any(2,3)</t>
+          <t>.any(2,3)</t>
         </is>
       </c>
     </row>
@@ -2267,7 +2259,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>qa2a.any(1,2)</t>
+          <t>qa2a.between(1:2)</t>
         </is>
       </c>
     </row>
@@ -2287,7 +2279,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>q12.any(2)</t>
+          <t>qa1.any(2)</t>
         </is>
       </c>
     </row>
@@ -2325,7 +2317,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>q1009.any(&lt;DGT0&gt;)</t>
+          <t>q1009.any()</t>
         </is>
       </c>
     </row>
@@ -2465,7 +2457,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>qf1.any(2)&amp;qf1.between.(</t>
+          <t>qa1.any(2)&amp;qa1.any(1)</t>
         </is>
       </c>
     </row>
@@ -2503,7 +2495,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>6611.any(&lt;DGT0&gt;)</t>
+          <t>6611.between(:)</t>
         </is>
       </c>
     </row>
@@ -2543,7 +2535,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>q28.any(&lt;DGT0&gt;)</t>
+          <t>q28.any()</t>
         </is>
       </c>
     </row>
@@ -2563,7 +2555,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>q1009.any(&lt;DGT0&gt;)</t>
+          <t>q1009.any()</t>
         </is>
       </c>
     </row>
@@ -2583,7 +2575,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>q6215.any(&lt;DGT0&gt;)</t>
+          <t>q6215.any(,)</t>
         </is>
       </c>
     </row>
@@ -2603,7 +2595,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>q6403.any(&lt;DGT0&gt;,&lt;DGT1&gt;)</t>
+          <t>q6403.any(,)</t>
         </is>
       </c>
     </row>
@@ -2623,7 +2615,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -2701,7 +2693,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>s2 &lt;18 or s2&gt;55</t>
+          <t>s2 &lt;18 or s2 &gt;55</t>
         </is>
       </c>
     </row>
@@ -2741,7 +2733,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>72000.any(&lt;DGT0&gt;)</t>
+          <t>72000.any()</t>
         </is>
       </c>
     </row>
@@ -2861,7 +2853,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>q102.any(1,2)</t>
+          <t>q102.any(1)</t>
         </is>
       </c>
     </row>
@@ -2919,7 +2911,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>1008.notany(5,&lt;DGT1&gt;)</t>
+          <t>1008.notany(5)</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2931,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>s1a.any(1)&amp;s1c.any(1)</t>
+          <t>s1a.any(1)</t>
         </is>
       </c>
     </row>
@@ -2977,7 +2969,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>1010.any(&lt;DGT0&gt;)</t>
+          <t>1010.any(,)</t>
         </is>
       </c>
     </row>
@@ -3017,7 +3009,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>q300001.any(&lt;DGT0&gt;)</t>
+          <t>q300001.between(:)</t>
         </is>
       </c>
     </row>
@@ -3037,7 +3029,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>q39.any(&lt;DGT0&gt;)</t>
+          <t>q39.any()</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3049,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>4006.any(&lt;DGT0&gt;)</t>
+          <t>4006.any()</t>
         </is>
       </c>
     </row>
@@ -3077,7 +3069,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>q1004.any(&lt;DGT0&gt;)</t>
+          <t>q1004.any()</t>
         </is>
       </c>
     </row>
@@ -3097,7 +3089,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>42061.any(1,4230)</t>
+          <t>42061.any(1)</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3109,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>qao.any(4)</t>
+          <t>.any(4)</t>
         </is>
       </c>
     </row>
@@ -3157,7 +3149,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>qa1.any(1,2)</t>
+          <t>qa1.any(1,2,3)</t>
         </is>
       </c>
     </row>
@@ -3177,7 +3169,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>20033.any(&lt;DGT0&gt;,&lt;DGT1&gt;,&lt;DGT2&gt;)</t>
+          <t>20033.any(,,,,)</t>
         </is>
       </c>
     </row>
@@ -3215,7 +3207,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>8010.notany(2,5)</t>
+          <t>8010.notany(2)</t>
         </is>
       </c>
     </row>
@@ -3235,7 +3227,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>qs10.any(1,2,3)&amp;qs11.any</t>
+          <t>qs3.any(1,2,3,16,4,5</t>
         </is>
       </c>
     </row>
@@ -3255,7 +3247,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>qd.any(1,4)</t>
+          <t>qd.between(1:4)</t>
         </is>
       </c>
     </row>
@@ -3393,7 +3385,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>6401.any(&lt;DGT0&gt;)</t>
+          <t>.any()</t>
         </is>
       </c>
     </row>
@@ -3433,7 +3425,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -3533,7 +3525,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>s4.any(02,03,04,06,07)</t>
+          <t>s4.any(02,03,04,06)</t>
         </is>
       </c>
     </row>
@@ -3553,7 +3545,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>1009.any(&lt;DGT0&gt;)</t>
+          <t>1009.any()</t>
         </is>
       </c>
     </row>
@@ -3613,7 +3605,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>q7702.any(&lt;DGT0&gt;,&lt;DGT1&gt;)</t>
+          <t>q7702.any()</t>
         </is>
       </c>
     </row>
@@ -3751,7 +3743,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -3771,7 +3763,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>d15.any(99)</t>
+          <t>d13.any(99)</t>
         </is>
       </c>
     </row>
@@ -3871,7 +3863,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>q115.notany(3,5)</t>
+          <t>q115.notany(3)</t>
         </is>
       </c>
     </row>
@@ -3891,7 +3883,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>14.any(&lt;DGT0&gt;)or q1002.any(&lt;DGT1&gt;)</t>
+          <t>14.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -3911,7 +3903,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>s10.any(4,5)</t>
+          <t>s10 &lt;4 or s10 &gt;5</t>
         </is>
       </c>
     </row>
@@ -3931,7 +3923,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>qa1.any(1,2)</t>
+          <t>qa1.any(1,2,3)</t>
         </is>
       </c>
     </row>
@@ -4071,7 +4063,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>q999901.any(3,4,5)</t>
+          <t>q999901.any(3,4)</t>
         </is>
       </c>
     </row>
@@ -4211,7 +4203,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>2226.any(&lt;DGT0&gt;)</t>
+          <t>2226.any()</t>
         </is>
       </c>
     </row>
@@ -4251,7 +4243,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>q10001.any(&lt;DGT0&gt;)</t>
+          <t>q10001.any()</t>
         </is>
       </c>
     </row>
@@ -4291,7 +4283,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>q1015.any(&lt;DGT0&gt;)</t>
+          <t>q1015.any()</t>
         </is>
       </c>
     </row>
@@ -4331,7 +4323,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>q15.any(1)</t>
+          <t>d12.any(1)</t>
         </is>
       </c>
     </row>
@@ -4351,7 +4343,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>qf1.between(1:2)&amp;..any(2</t>
+          <t>qf1.any(1,2,3)</t>
         </is>
       </c>
     </row>
@@ -4411,7 +4403,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>q600001.any(&lt;DGT0&gt;)</t>
+          <t>q600001.any()</t>
         </is>
       </c>
     </row>
@@ -4431,7 +4423,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>8042.between(1:2,3)&amp;8050.between</t>
+          <t>8012.any(1,2,3,4,).</t>
         </is>
       </c>
     </row>
@@ -4469,7 +4461,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>q1011.any(&lt;DGT0&gt;,&lt;DGT1&gt;)</t>
+          <t>q1011.any(,,)</t>
         </is>
       </c>
     </row>
@@ -4489,7 +4481,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>1.any(&lt;DGT0&gt;)</t>
+          <t>1.any()</t>
         </is>
       </c>
     </row>
@@ -4509,7 +4501,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>qd.any(1,4)</t>
+          <t>qd.between(1:4)</t>
         </is>
       </c>
     </row>
@@ -4569,7 +4561,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>q1004.any(&lt;DGT0&gt;)</t>
+          <t>q1004.any()</t>
         </is>
       </c>
     </row>
@@ -4669,7 +4661,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>&lt;QID2&gt;.between(1:3)</t>
+          <t>q2202.any(1,3)</t>
         </is>
       </c>
     </row>
@@ -4709,7 +4701,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>.any(4)</t>
+          <t>1042.any(4)</t>
         </is>
       </c>
     </row>
@@ -4749,7 +4741,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>2006.any(&lt;DGT0&gt;)</t>
+          <t>2006.any()</t>
         </is>
       </c>
     </row>
@@ -4787,7 +4779,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>5000.notanswered(1)</t>
+          <t>5000.answered(1)</t>
         </is>
       </c>
     </row>
@@ -4827,7 +4819,7 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>qd2.any(2)&amp;qd2.any(2)</t>
+          <t>qa1.any(2)&amp;qa1.any(7)</t>
         </is>
       </c>
     </row>
@@ -4847,7 +4839,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>qg1.any(1,6)</t>
+          <t>qg1.between(1:6)</t>
         </is>
       </c>
     </row>
@@ -4927,7 +4919,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -4965,7 +4957,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>q1011.notany(&lt;DGT0&gt;,&lt;DGT1&gt;)</t>
+          <t>q1011.any(,,)</t>
         </is>
       </c>
     </row>
@@ -4985,7 +4977,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>s4a &lt;3 or s4a&gt;30</t>
+          <t>s4a &lt;3 or s4a &gt;30</t>
         </is>
       </c>
     </row>
@@ -5025,7 +5017,7 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>q1201.any(&lt;DGT0&gt;)</t>
+          <t>q1201.notany()</t>
         </is>
       </c>
     </row>
@@ -5045,7 +5037,7 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>qa1.any(3,5)</t>
+          <t>qa1.between(3:5)</t>
         </is>
       </c>
     </row>
@@ -5085,7 +5077,7 @@
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>q102.any(1,2)</t>
+          <t>q102.any(1)</t>
         </is>
       </c>
     </row>
@@ -5125,7 +5117,7 @@
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>q9.any(1)&amp;a10.any(1)</t>
+          <t>q9.any(1)</t>
         </is>
       </c>
     </row>
@@ -5185,7 +5177,7 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>qd.between(5:9)</t>
+          <t>q25a.any(5,9)</t>
         </is>
       </c>
     </row>
@@ -5205,7 +5197,7 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>qr7.any(1)&amp;qr7.any(1)</t>
+          <t>q30.any(1)&amp;q30.any(4)</t>
         </is>
       </c>
     </row>
@@ -5245,7 +5237,7 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>q115.any(3,5)</t>
+          <t>q115.notany(3,5)</t>
         </is>
       </c>
     </row>
@@ -5265,7 +5257,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>qd.any(1,4)</t>
+          <t>qd.between(1:4)</t>
         </is>
       </c>
     </row>
@@ -5387,7 +5379,7 @@
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>s3.any(1,2,3)</t>
+          <t>3.any(1,2)&amp;s3.any(3</t>
         </is>
       </c>
     </row>
@@ -5407,7 +5399,7 @@
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>4230.any(&lt;DGT0&gt;)</t>
+          <t>4230.any()</t>
         </is>
       </c>
     </row>
@@ -5427,7 +5419,7 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>q9av1.any(1,2)</t>
+          <t>q9av1.between(1:2)</t>
         </is>
       </c>
     </row>
@@ -5447,7 +5439,7 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>s3.any(3,4,&lt;DGT2&gt;)</t>
+          <t>s3.any(3,4)</t>
         </is>
       </c>
     </row>
@@ -5485,7 +5477,7 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>1007.any(4)</t>
+          <t>1007.notany(4)</t>
         </is>
       </c>
     </row>
@@ -5605,7 +5597,7 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>qa1.any(2)&amp;qd2.between.between(7</t>
+          <t>qa1.any(2)&amp;qa1.any(7)</t>
         </is>
       </c>
     </row>
@@ -5645,7 +5637,7 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>2006.any(&lt;DGT0&gt;)</t>
+          <t>2006.any()</t>
         </is>
       </c>
     </row>
@@ -5725,7 +5717,7 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>s3_s3.any(25)</t>
+          <t>s3.any(25)</t>
         </is>
       </c>
     </row>
@@ -5745,7 +5737,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>s5.any(2,35)</t>
+          <t>s5 &lt;2 or s5 &gt;35</t>
         </is>
       </c>
     </row>
@@ -5765,7 +5757,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>q1.notany(7)or q2.between.between(1</t>
+          <t>q1.any(7)or q2.any(1)</t>
         </is>
       </c>
     </row>
@@ -5805,7 +5797,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>qd.any(1,4)</t>
+          <t>qd.between(1:4)</t>
         </is>
       </c>
     </row>
@@ -5944,7 +5936,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>&lt;QID3&gt;.any(&lt;DGT0&gt;)or q99009.</t>
+          <t>q1002.any()</t>
         </is>
       </c>
     </row>
@@ -5964,7 +5956,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>question2.notbetween(18:75)</t>
+          <t>question2.notany(18)</t>
         </is>
       </c>
     </row>
@@ -6022,7 +6014,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>5000.notanswered(1)</t>
+          <t>5000.answered(1)</t>
         </is>
       </c>
     </row>
@@ -6042,7 +6034,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>q1011.any(1,2)&amp;q1013.between.between</t>
+          <t>q1011.any(1,2,3)</t>
         </is>
       </c>
     </row>
@@ -6062,7 +6054,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>&lt;DGT1&gt;.any(10)</t>
+          <t>q8015.any(10)</t>
         </is>
       </c>
     </row>
@@ -6082,7 +6074,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>q1018.any(&lt;DGT0&gt;)</t>
+          <t>q1018.notany()</t>
         </is>
       </c>
     </row>
@@ -6102,7 +6094,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>q6203.any(&lt;DGT0&gt;,&lt;DGT1&gt;)</t>
+          <t>q6203.any(,)</t>
         </is>
       </c>
     </row>
@@ -6140,7 +6132,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>s11.notany(3)or &lt;QID2&gt;.between.(5:</t>
+          <t>s11.notany(3)</t>
         </is>
       </c>
     </row>
@@ -6160,7 +6152,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>q.between(1:2)</t>
+          <t>q.any(1)</t>
         </is>
       </c>
     </row>
@@ -6201,7 +6193,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>s3.between(3:30)</t>
+          <t>s2.between(3:30)</t>
         </is>
       </c>
     </row>
@@ -6221,7 +6213,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>q115.notany(3,5)</t>
+          <t>q115.notany(3)</t>
         </is>
       </c>
     </row>
@@ -6261,7 +6253,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>s4.any(80)</t>
+          <t>s4.between(80:)</t>
         </is>
       </c>
     </row>
@@ -6279,7 +6271,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>&lt;QID1&gt;.any(1,3)</t>
+          <t>.any(1,3)</t>
         </is>
       </c>
     </row>
@@ -6357,7 +6349,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>8010.notany(18)</t>
+          <t>8010&lt;18 or 8010&gt;65</t>
         </is>
       </c>
     </row>
@@ -6457,7 +6449,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>qa6a.any(1,2)</t>
+          <t>qa6a.any(1)</t>
         </is>
       </c>
     </row>
@@ -6515,7 +6507,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>s2 &lt;18 or s2&gt;55</t>
+          <t>s2 &lt;18 or s2 &gt;55</t>
         </is>
       </c>
     </row>
@@ -6675,7 +6667,7 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>2006.any(&lt;DGT0&gt;)</t>
+          <t>2006.any()</t>
         </is>
       </c>
     </row>
@@ -6735,7 +6727,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>qa1.any(2)&amp;qd3.any(2)</t>
+          <t>qa1.any(2)&amp;qd2.any(7)</t>
         </is>
       </c>
     </row>
@@ -6815,7 +6807,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -6855,7 +6847,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>qa.any(2)&amp;qg1.between.(1:</t>
+          <t>qa.any(2)&amp;qg2.any(1)</t>
         </is>
       </c>
     </row>
@@ -6895,7 +6887,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>q7701.any(&lt;DGT0&gt;,&lt;DGT1&gt;)</t>
+          <t>q7701.between(:)</t>
         </is>
       </c>
     </row>
@@ -6955,7 +6947,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>s2 &lt;18 or s2&gt;55</t>
+          <t>s2 &lt;18 or s2 &gt;55</t>
         </is>
       </c>
     </row>
@@ -7031,11 +7023,7 @@
           <t>Younger than 18 years TERM</t>
         </is>
       </c>
-      <c r="D336" t="inlineStr">
-        <is>
-          <t>8017&lt;18</t>
-        </is>
-      </c>
+      <c r="D336" t="inlineStr"/>
     </row>
     <row r="337">
       <c r="A337" s="1" t="n">
@@ -7053,7 +7041,7 @@
       </c>
       <c r="D337" t="inlineStr">
         <is>
-          <t>q00012.any(&lt;DGT0&gt;)</t>
+          <t>q00012.any()</t>
         </is>
       </c>
     </row>
@@ -7073,7 +7061,7 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>8400.any(&lt;DGT0&gt;)</t>
+          <t>8400.any()</t>
         </is>
       </c>
     </row>
@@ -7091,7 +7079,7 @@
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>1401.answered()</t>
+          <t>.answered(1)</t>
         </is>
       </c>
     </row>
@@ -7151,7 +7139,7 @@
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>1300.any(4,5,1)</t>
+          <t>1300.any(4,5,1,2)</t>
         </is>
       </c>
     </row>
@@ -7191,7 +7179,7 @@
       </c>
       <c r="D344" t="inlineStr">
         <is>
-          <t>q1009.any(&lt;DGT0&gt;,&lt;DGT1&gt;,&lt;DGT2&gt;)</t>
+          <t>q1009.any(,,,,)</t>
         </is>
       </c>
     </row>
@@ -7251,7 +7239,7 @@
       </c>
       <c r="D347" t="inlineStr">
         <is>
-          <t>s5.any(2,35)</t>
+          <t>s5 &lt;2 or s5 &gt;35</t>
         </is>
       </c>
     </row>
@@ -7271,7 +7259,7 @@
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>d9.between(99:11)</t>
+          <t>d9.any(11,)</t>
         </is>
       </c>
     </row>
@@ -7291,7 +7279,7 @@
       </c>
       <c r="D349" t="inlineStr">
         <is>
-          <t>q6.between(6:&lt;DGT1&gt;)</t>
+          <t>q6.any(,)</t>
         </is>
       </c>
     </row>
@@ -7311,7 +7299,7 @@
       </c>
       <c r="D350" t="inlineStr">
         <is>
-          <t>qd.any(1)</t>
+          <t>qa1.any(1)</t>
         </is>
       </c>
     </row>
@@ -7331,7 +7319,7 @@
       </c>
       <c r="D351" t="inlineStr">
         <is>
-          <t>2302b.notany(3)</t>
+          <t>q2202.any(3)</t>
         </is>
       </c>
     </row>
@@ -7431,7 +7419,7 @@
       </c>
       <c r="D356" t="inlineStr">
         <is>
-          <t>q1004.notany(1,2)</t>
+          <t>q1004.notany(1)</t>
         </is>
       </c>
     </row>
@@ -7511,7 +7499,7 @@
       </c>
       <c r="D360" t="inlineStr">
         <is>
-          <t>qd.any(1,4)</t>
+          <t>qd.between(1:4)</t>
         </is>
       </c>
     </row>
@@ -7531,7 +7519,7 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>cell.between(1:&lt;DGT1&gt;)</t>
+          <t>cell.any(1)</t>
         </is>
       </c>
     </row>
@@ -7571,7 +7559,7 @@
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>q10.any(1)&amp;.between.(2)</t>
+          <t>q9.any(1)&amp;q9.any(2)</t>
         </is>
       </c>
     </row>
@@ -7591,7 +7579,7 @@
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>1010.any(&lt;DGT0&gt;)</t>
+          <t>1010.any(,)</t>
         </is>
       </c>
     </row>
@@ -7611,7 +7599,7 @@
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>s4 &lt;2 or s4&gt;38</t>
+          <t>s4&lt;2 or s4&gt;38</t>
         </is>
       </c>
     </row>
@@ -7651,7 +7639,7 @@
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>&lt;QID2&gt;.any(1)</t>
+          <t>q1.between(1:2)</t>
         </is>
       </c>
     </row>
@@ -7691,7 +7679,7 @@
       </c>
       <c r="D369" t="inlineStr">
         <is>
-          <t>qs11.any(9)</t>
+          <t>qs10.any(9)</t>
         </is>
       </c>
     </row>
@@ -7711,7 +7699,7 @@
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>qa1.any(2)&amp;qd2.between.between(7</t>
+          <t>qa1.any(2)&amp;qa1.any(7)</t>
         </is>
       </c>
     </row>
@@ -7731,7 +7719,7 @@
       </c>
       <c r="D371" t="inlineStr">
         <is>
-          <t>qc1.any(1,2)</t>
+          <t>qa1.any(1,2,3)</t>
         </is>
       </c>
     </row>
@@ -7791,7 +7779,7 @@
       </c>
       <c r="D374" t="inlineStr">
         <is>
-          <t>q071.any(&lt;DGT0&gt;)</t>
+          <t>q071.any()</t>
         </is>
       </c>
     </row>
@@ -7889,7 +7877,7 @@
       </c>
       <c r="D379" t="inlineStr">
         <is>
-          <t>..any(3)</t>
+          <t>.any(3)</t>
         </is>
       </c>
     </row>
@@ -7909,7 +7897,7 @@
       </c>
       <c r="D380" t="inlineStr">
         <is>
-          <t>q1011.any(1,2,3)&amp;q1013.any</t>
+          <t>q1011.any(1,2,3,10)</t>
         </is>
       </c>
     </row>
@@ -7949,7 +7937,7 @@
       </c>
       <c r="D382" t="inlineStr">
         <is>
-          <t>.any(&lt;DGT0&gt;)</t>
+          <t>.any()</t>
         </is>
       </c>
     </row>
@@ -7969,7 +7957,7 @@
       </c>
       <c r="D383" t="inlineStr">
         <is>
-          <t>s4 &lt;2 or s4&gt;38</t>
+          <t>s4&lt;2 or s4&gt;38</t>
         </is>
       </c>
     </row>
@@ -8109,7 +8097,7 @@
       </c>
       <c r="D390" t="inlineStr">
         <is>
-          <t>219621.any(&lt;DGT0&gt;)</t>
+          <t>219621.any()</t>
         </is>
       </c>
     </row>
@@ -8149,7 +8137,7 @@
       </c>
       <c r="D392" t="inlineStr">
         <is>
-          <t>.any(&lt;DGT0&gt;,&lt;DGT1&gt;)</t>
+          <t>.any()</t>
         </is>
       </c>
     </row>
@@ -8189,7 +8177,7 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>qao.any(2)</t>
+          <t>.any(2)</t>
         </is>
       </c>
     </row>
@@ -8227,7 +8215,7 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>00012.answered()</t>
+          <t>00012.answered(1)</t>
         </is>
       </c>
     </row>
@@ -8287,7 +8275,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>qa1.any(2)&amp;qd2.between.between(7</t>
+          <t>qa1.any(2)&amp;qa1.any(7)</t>
         </is>
       </c>
     </row>
@@ -8387,7 +8375,7 @@
       </c>
       <c r="D404" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -8407,7 +8395,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -8527,7 +8515,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>ml03.any(2,7)</t>
+          <t>ml03.between(2:7)</t>
         </is>
       </c>
     </row>
@@ -8683,7 +8671,7 @@
       </c>
       <c r="D419" t="inlineStr">
         <is>
-          <t>1008.notany(&lt;DGT0&gt;,&lt;DGT1&gt;)</t>
+          <t>1008.notany(,)</t>
         </is>
       </c>
     </row>
@@ -8743,7 +8731,7 @@
       </c>
       <c r="D422" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -8763,7 +8751,7 @@
       </c>
       <c r="D423" t="inlineStr">
         <is>
-          <t>q105b.any(1,12)</t>
+          <t>q105b.any(1)</t>
         </is>
       </c>
     </row>
@@ -8803,7 +8791,7 @@
       </c>
       <c r="D425" t="inlineStr">
         <is>
-          <t>q300001.any(&lt;DGT0&gt;)</t>
+          <t>q300001.any()</t>
         </is>
       </c>
     </row>
@@ -8823,7 +8811,7 @@
       </c>
       <c r="D426" t="inlineStr">
         <is>
-          <t>4051.any(&lt;DGT0&gt;,&lt;DGT1&gt;)</t>
+          <t>4051.any(,)</t>
         </is>
       </c>
     </row>
@@ -8863,7 +8851,7 @@
       </c>
       <c r="D428" t="inlineStr">
         <is>
-          <t>q15a.between(1:4)</t>
+          <t>qd.between(1:4)</t>
         </is>
       </c>
     </row>
@@ -8883,7 +8871,7 @@
       </c>
       <c r="D429" t="inlineStr">
         <is>
-          <t>qa1.any(2)&amp;qd2.between.any(7</t>
+          <t>qa1.any(2)&amp;qd2.any(7)</t>
         </is>
       </c>
     </row>
@@ -8943,7 +8931,7 @@
       </c>
       <c r="D432" t="inlineStr">
         <is>
-          <t>s7.any(75)</t>
+          <t>s7&lt;75</t>
         </is>
       </c>
     </row>
@@ -9001,7 +8989,7 @@
       </c>
       <c r="D435" t="inlineStr">
         <is>
-          <t>s3.any(3,4,&lt;DGT2&gt;)</t>
+          <t>s3.any(3,4)</t>
         </is>
       </c>
     </row>
@@ -9021,7 +9009,7 @@
       </c>
       <c r="D436" t="inlineStr">
         <is>
-          <t>q6611.any(&lt;DGT0&gt;)</t>
+          <t>q6611.between(:)</t>
         </is>
       </c>
     </row>
@@ -9041,7 +9029,7 @@
       </c>
       <c r="D437" t="inlineStr">
         <is>
-          <t>qa1.any(2)&amp;qd2.between.between(7</t>
+          <t>qa1.any(2)&amp;qd2.any(7)</t>
         </is>
       </c>
     </row>
@@ -9061,7 +9049,7 @@
       </c>
       <c r="D438" t="inlineStr">
         <is>
-          <t>00020.any(4)&amp;00020.any(4)</t>
+          <t>00016.any(4)&amp;00016.any(6)</t>
         </is>
       </c>
     </row>
@@ -9081,7 +9069,7 @@
       </c>
       <c r="D439" t="inlineStr">
         <is>
-          <t>q7703.any(&lt;DGT0&gt;,&lt;DGT1&gt;)</t>
+          <t>q7703.between(:)</t>
         </is>
       </c>
     </row>
@@ -9121,7 +9109,7 @@
       </c>
       <c r="D441" t="inlineStr">
         <is>
-          <t>q102.any(1,2)</t>
+          <t>q102.any(1)</t>
         </is>
       </c>
     </row>
@@ -9161,7 +9149,7 @@
       </c>
       <c r="D443" t="inlineStr">
         <is>
-          <t>qa1.any(1,2)</t>
+          <t>qa1.any(1,2,3)</t>
         </is>
       </c>
     </row>
@@ -9299,7 +9287,7 @@
       </c>
       <c r="D450" t="inlineStr">
         <is>
-          <t>cc07.any(1,5)</t>
+          <t>cc07.between(1:5)</t>
         </is>
       </c>
     </row>
@@ -9357,7 +9345,7 @@
       </c>
       <c r="D453" t="inlineStr">
         <is>
-          <t>q1008.any(&lt;DGT0&gt;,&lt;DGT1&gt;)</t>
+          <t>q1008.notany(,)</t>
         </is>
       </c>
     </row>
@@ -9377,7 +9365,7 @@
       </c>
       <c r="D454" t="inlineStr">
         <is>
-          <t>22016.any(&lt;DGT0&gt;)</t>
+          <t>22016.any()</t>
         </is>
       </c>
     </row>
@@ -9417,7 +9405,7 @@
       </c>
       <c r="D456" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -9437,7 +9425,7 @@
       </c>
       <c r="D457" t="inlineStr">
         <is>
-          <t>cell.between(2:&lt;DGT1&gt;)</t>
+          <t>cell.any(2)</t>
         </is>
       </c>
     </row>
@@ -9577,7 +9565,7 @@
       </c>
       <c r="D464" t="inlineStr">
         <is>
-          <t>q4.notanswered(1)</t>
+          <t>q4.notbetween(1:)</t>
         </is>
       </c>
     </row>
@@ -9617,7 +9605,7 @@
       </c>
       <c r="D466" t="inlineStr">
         <is>
-          <t>s2 &lt;18 or s2&gt;55</t>
+          <t>s2 &lt;18 or s2 &gt;55</t>
         </is>
       </c>
     </row>
@@ -9637,7 +9625,7 @@
       </c>
       <c r="D467" t="inlineStr">
         <is>
-          <t>q1016.any(&lt;DGT0&gt;)</t>
+          <t>..any()</t>
         </is>
       </c>
     </row>
@@ -9733,7 +9721,7 @@
       </c>
       <c r="D472" t="inlineStr">
         <is>
-          <t>&lt;QID2&gt;.any(2)</t>
+          <t>qa1.any(2)</t>
         </is>
       </c>
     </row>
@@ -9751,7 +9739,7 @@
       </c>
       <c r="D473" t="inlineStr">
         <is>
-          <t>8010&lt;16 or 8010&gt;34</t>
+          <t>8010&lt;16</t>
         </is>
       </c>
     </row>
@@ -9771,7 +9759,7 @@
       </c>
       <c r="D474" t="inlineStr">
         <is>
-          <t>b5d.any(1,2)</t>
+          <t>b5d.any(2,,)</t>
         </is>
       </c>
     </row>
@@ -9791,7 +9779,7 @@
       </c>
       <c r="D475" t="inlineStr">
         <is>
-          <t>qa2a.any(1,2)</t>
+          <t>qa2a.between(1:2)</t>
         </is>
       </c>
     </row>
@@ -9809,7 +9797,7 @@
       </c>
       <c r="D476" t="inlineStr">
         <is>
-          <t>8010.notbetween(34:&lt;DGT1&gt;)</t>
+          <t>8010.notbetween(34)</t>
         </is>
       </c>
     </row>
@@ -9829,7 +9817,7 @@
       </c>
       <c r="D477" t="inlineStr">
         <is>
-          <t>4006.any(&lt;DGT0&gt;)</t>
+          <t>4006.any()</t>
         </is>
       </c>
     </row>
@@ -10049,7 +10037,7 @@
       </c>
       <c r="D488" t="inlineStr">
         <is>
-          <t>22.notany(2)</t>
+          <t>22.between(2:)</t>
         </is>
       </c>
     </row>
@@ -10089,7 +10077,7 @@
       </c>
       <c r="D490" t="inlineStr">
         <is>
-          <t>00020.any(4)&amp;00020.any(4)</t>
+          <t>00016.any(4)&amp;00016.any(6)</t>
         </is>
       </c>
     </row>
@@ -10109,7 +10097,7 @@
       </c>
       <c r="D491" t="inlineStr">
         <is>
-          <t>cc07.any(1,5)</t>
+          <t>cc07.between(1:5)</t>
         </is>
       </c>
     </row>
@@ -10149,7 +10137,7 @@
       </c>
       <c r="D493" t="inlineStr">
         <is>
-          <t>s5.any(2,35)</t>
+          <t>s5 &lt;2 or s5 &gt;35</t>
         </is>
       </c>
     </row>
@@ -10209,7 +10197,7 @@
       </c>
       <c r="D496" t="inlineStr">
         <is>
-          <t>q6501.any(&lt;DGT0&gt;,&lt;DGT1&gt;)</t>
+          <t>q6501.any(,)</t>
         </is>
       </c>
     </row>
@@ -10329,7 +10317,7 @@
       </c>
       <c r="D502" t="inlineStr">
         <is>
-          <t>q3260.any(&lt;DGT0&gt;)</t>
+          <t>q3260.any()</t>
         </is>
       </c>
     </row>
@@ -10369,7 +10357,7 @@
       </c>
       <c r="D504" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q88001.</t>
+          <t>.any()</t>
         </is>
       </c>
     </row>
@@ -10389,7 +10377,7 @@
       </c>
       <c r="D505" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -10469,7 +10457,7 @@
       </c>
       <c r="D509" t="inlineStr">
         <is>
-          <t>cc07.any(1,5)</t>
+          <t>cc07.between(1:5)</t>
         </is>
       </c>
     </row>
@@ -10509,7 +10497,7 @@
       </c>
       <c r="D511" t="inlineStr">
         <is>
-          <t>s3 &lt;25 or s3&gt;54</t>
+          <t>s3 &lt;25 or s3 &gt;54</t>
         </is>
       </c>
     </row>
@@ -10529,7 +10517,7 @@
       </c>
       <c r="D512" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -10549,7 +10537,7 @@
       </c>
       <c r="D513" t="inlineStr">
         <is>
-          <t>&lt;QID2&gt;.any(1,3)</t>
+          <t>q2203.any(1,3)</t>
         </is>
       </c>
     </row>
@@ -10669,7 +10657,7 @@
       </c>
       <c r="D519" t="inlineStr">
         <is>
-          <t>q6215.any(&lt;DGT0&gt;)</t>
+          <t>q6215.any(,)</t>
         </is>
       </c>
     </row>
@@ -10747,7 +10735,7 @@
       </c>
       <c r="D523" t="inlineStr">
         <is>
-          <t>801256.any(&lt;DGT0&gt;)</t>
+          <t>.any(,)</t>
         </is>
       </c>
     </row>
@@ -10767,7 +10755,7 @@
       </c>
       <c r="D524" t="inlineStr">
         <is>
-          <t>q115.any(3,5)</t>
+          <t>q115.notany(3,5)</t>
         </is>
       </c>
     </row>
@@ -10787,7 +10775,7 @@
       </c>
       <c r="D525" t="inlineStr">
         <is>
-          <t>q2250.any(&lt;DGT0&gt;)</t>
+          <t>q2250.any()</t>
         </is>
       </c>
     </row>
@@ -10807,7 +10795,7 @@
       </c>
       <c r="D526" t="inlineStr">
         <is>
-          <t>qa1.any(2)&amp;qd2.between.between(7</t>
+          <t>qa1.any(2)&amp;qa1.any(7)</t>
         </is>
       </c>
     </row>
@@ -10827,7 +10815,7 @@
       </c>
       <c r="D527" t="inlineStr">
         <is>
-          <t>q6.notanswered(1)</t>
+          <t>q6.answered(1)</t>
         </is>
       </c>
     </row>
@@ -10905,7 +10893,7 @@
       </c>
       <c r="D531" t="inlineStr">
         <is>
-          <t>qintro8.any(5,1)</t>
+          <t>qintro8.between(5:1)</t>
         </is>
       </c>
     </row>
@@ -10945,7 +10933,7 @@
       </c>
       <c r="D533" t="inlineStr">
         <is>
-          <t>&lt;DGT2&gt;.any(2,3)</t>
+          <t>.any(2,3)</t>
         </is>
       </c>
     </row>
@@ -10985,7 +10973,7 @@
       </c>
       <c r="D535" t="inlineStr">
         <is>
-          <t>q6225.any(&lt;DGT0&gt;)</t>
+          <t>q6225.any()</t>
         </is>
       </c>
     </row>
@@ -11025,7 +11013,7 @@
       </c>
       <c r="D537" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -11065,7 +11053,7 @@
       </c>
       <c r="D539" t="inlineStr">
         <is>
-          <t>q1201.any(&lt;DGT0&gt;)</t>
+          <t>q1201.any()</t>
         </is>
       </c>
     </row>
@@ -11103,7 +11091,7 @@
       </c>
       <c r="D541" t="inlineStr">
         <is>
-          <t>2001.answered()</t>
+          <t>2001.answered(1)</t>
         </is>
       </c>
     </row>
@@ -11123,7 +11111,7 @@
       </c>
       <c r="D542" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)</t>
+          <t>q1002.any()</t>
         </is>
       </c>
     </row>
@@ -11203,7 +11191,7 @@
       </c>
       <c r="D546" t="inlineStr">
         <is>
-          <t>q1009.any(&lt;DGT0&gt;)</t>
+          <t>q1009.any()</t>
         </is>
       </c>
     </row>
@@ -11243,7 +11231,7 @@
       </c>
       <c r="D548" t="inlineStr">
         <is>
-          <t>q1.notany(7)or q2.between.between(1</t>
+          <t>q1.any(7)or q2.any(1)</t>
         </is>
       </c>
     </row>
@@ -11283,7 +11271,7 @@
       </c>
       <c r="D550" t="inlineStr">
         <is>
-          <t>&lt;QID2&gt;.any(2)</t>
+          <t>qa1.any(2)</t>
         </is>
       </c>
     </row>
@@ -11323,7 +11311,7 @@
       </c>
       <c r="D552" t="inlineStr">
         <is>
-          <t>s5.any(2,35)</t>
+          <t>s5 &lt;2 or s5 &gt;35</t>
         </is>
       </c>
     </row>
@@ -11423,7 +11411,7 @@
       </c>
       <c r="D557" t="inlineStr">
         <is>
-          <t>qd.any(1,5)</t>
+          <t>qd.between(1:5)</t>
         </is>
       </c>
     </row>
@@ -11523,7 +11511,7 @@
       </c>
       <c r="D562" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -11563,7 +11551,7 @@
       </c>
       <c r="D564" t="inlineStr">
         <is>
-          <t>q6225.any(&lt;DGT0&gt;)</t>
+          <t>q6225.any()</t>
         </is>
       </c>
     </row>
@@ -11581,7 +11569,7 @@
       </c>
       <c r="D565" t="inlineStr">
         <is>
-          <t>8010&lt;18</t>
+          <t>&lt;18</t>
         </is>
       </c>
     </row>
@@ -11601,7 +11589,7 @@
       </c>
       <c r="D566" t="inlineStr">
         <is>
-          <t>qa1.any(1,2)</t>
+          <t>qa1.any(1,2,3)</t>
         </is>
       </c>
     </row>
@@ -11621,7 +11609,7 @@
       </c>
       <c r="D567" t="inlineStr">
         <is>
-          <t>q223.any(1,2,3)</t>
+          <t>q223.any(1,2)</t>
         </is>
       </c>
     </row>
@@ -11641,7 +11629,7 @@
       </c>
       <c r="D568" t="inlineStr">
         <is>
-          <t>qa1.between(3:5)</t>
+          <t>.between(3:5)</t>
         </is>
       </c>
     </row>
@@ -11661,7 +11649,7 @@
       </c>
       <c r="D569" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -11681,7 +11669,7 @@
       </c>
       <c r="D570" t="inlineStr">
         <is>
-          <t>q9.any(1)&amp;q10.between.between(2</t>
+          <t>q9.any(1)&amp;q10.between(2:5</t>
         </is>
       </c>
     </row>
@@ -11721,7 +11709,7 @@
       </c>
       <c r="D572" t="inlineStr">
         <is>
-          <t>q1002.any(&lt;DGT0&gt;)or q1003.any(&lt;DGT1&gt;)</t>
+          <t>q1002.any()or .any()</t>
         </is>
       </c>
     </row>
@@ -11781,7 +11769,7 @@
       </c>
       <c r="D575" t="inlineStr">
         <is>
-          <t>q016.any(&lt;DGT0&gt;,&lt;DGT1&gt;)</t>
+          <t>q016.any(,)</t>
         </is>
       </c>
     </row>
@@ -11801,7 +11789,7 @@
       </c>
       <c r="D576" t="inlineStr">
         <is>
-          <t>22.notany(2)</t>
+          <t>22.between(2:)</t>
         </is>
       </c>
     </row>
@@ -11841,7 +11829,7 @@
       </c>
       <c r="D578" t="inlineStr">
         <is>
-          <t>q9999.any(&lt;DGT0&gt;,&lt;DGT1&gt;,&lt;DGT2&gt;,&lt;DGT3&gt;)</t>
+          <t>q9999.any(,,,)</t>
         </is>
       </c>
     </row>
@@ -11861,7 +11849,7 @@
       </c>
       <c r="D579" t="inlineStr">
         <is>
-          <t>42016.any(&lt;DGT0&gt;)</t>
+          <t>42016.any()</t>
         </is>
       </c>
     </row>
@@ -11901,7 +11889,7 @@
       </c>
       <c r="D581" t="inlineStr">
         <is>
-          <t>d9.any(99,11)</t>
+          <t>d9.any(11,)</t>
         </is>
       </c>
     </row>
@@ -11921,7 +11909,7 @@
       </c>
       <c r="D582" t="inlineStr">
         <is>
-          <t>q5.notanswered(1)</t>
+          <t>q5.notbetween(1:)</t>
         </is>
       </c>
     </row>
@@ -11941,7 +11929,7 @@
       </c>
       <c r="D583" t="inlineStr">
         <is>
-          <t>q42061.any(&lt;DGT0&gt;)</t>
+          <t>q42061.any()</t>
         </is>
       </c>
     </row>
@@ -11981,7 +11969,7 @@
       </c>
       <c r="D585" t="inlineStr">
         <is>
-          <t>s2.notany(5,6,7)</t>
+          <t>s2.notany(5,6)</t>
         </is>
       </c>
     </row>
@@ -12021,7 +12009,7 @@
       </c>
       <c r="D587" t="inlineStr">
         <is>
-          <t>3101.any(1)&amp;3301.any(1)</t>
+          <t>3101.any(1,2)</t>
         </is>
       </c>
     </row>
@@ -12061,7 +12049,7 @@
       </c>
       <c r="D589" t="inlineStr">
         <is>
-          <t>&lt;QID2&gt;.any(1)</t>
+          <t>s9.any(1)</t>
         </is>
       </c>
     </row>

</xml_diff>